<commit_message>
ultimo commit pre banca
</commit_message>
<xml_diff>
--- a/Output de dados/erros_viagens_ODS.xlsx
+++ b/Output de dados/erros_viagens_ODS.xlsx
@@ -438,7 +438,7 @@
         <v>0.01105416924278444</v>
       </c>
       <c r="F2">
-        <v>0.0108479684578334</v>
+        <v>0.01084822484753873</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -458,7 +458,7 @@
         <v>0.03462655354126155</v>
       </c>
       <c r="F3">
-        <v>0.03543947694459991</v>
+        <v>0.0354396496667474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>